<commit_message>
Updated to put an image on every page of the word doc.
</commit_message>
<xml_diff>
--- a/Content/info.xlsx
+++ b/Content/info.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hello" sheetId="1" r:id="R84d74b56b9cb4781"/>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="studentlist" sheetId="2" r:id="R23eeb85480f54fd4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hello" sheetId="1" r:id="Rd321c984e0d9443d"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="studentlist" sheetId="2" r:id="R96f1d8196683452a"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -35,7 +35,7 @@
     <x:t>Age</x:t>
   </x:si>
   <x:si>
-    <x:t>849e0219-248b-4a47-8f98-6a6678e1ee47</x:t>
+    <x:t>346d2b26-6230-4a53-88b3-c13234a4c614</x:t>
   </x:si>
   <x:si>
     <x:t>20033515</x:t>
@@ -56,7 +56,7 @@
     <x:t>48</x:t>
   </x:si>
   <x:si>
-    <x:t>bae3426f-5bdd-4f98-8132-f4308fa346a2</x:t>
+    <x:t>9437ad37-acd4-426b-896a-b81d6cd9fb4b</x:t>
   </x:si>
   <x:si>
     <x:t>200423859</x:t>
@@ -74,7 +74,7 @@
     <x:t>42</x:t>
   </x:si>
   <x:si>
-    <x:t>c5000072-146f-4531-865f-97183641e93b</x:t>
+    <x:t>f1565c3c-ae13-46c6-ac2f-f9ed5d6c1d3a</x:t>
   </x:si>
   <x:si>
     <x:t>200425031</x:t>
@@ -92,7 +92,7 @@
     <x:t>29</x:t>
   </x:si>
   <x:si>
-    <x:t>268c22cb-397a-4dfa-9110-0cabc37c411b</x:t>
+    <x:t>635b31a4-2ca7-4105-bc6d-53030a6251d0</x:t>
   </x:si>
   <x:si>
     <x:t>200425170</x:t>
@@ -110,7 +110,7 @@
     <x:t>28</x:t>
   </x:si>
   <x:si>
-    <x:t>261fda56-aa3c-4117-a63d-27d86131640a</x:t>
+    <x:t>cebe5710-2844-4c0d-9a61-33f09ae35d97</x:t>
   </x:si>
   <x:si>
     <x:t>200425198</x:t>
@@ -128,7 +128,7 @@
     <x:t>23</x:t>
   </x:si>
   <x:si>
-    <x:t>8cd3ea88-ebd3-4081-bb17-93afe34c031f</x:t>
+    <x:t>c5b96f69-4700-459d-8b6b-6cfc508647a6</x:t>
   </x:si>
   <x:si>
     <x:t>200427977</x:t>
@@ -146,7 +146,7 @@
     <x:t>25</x:t>
   </x:si>
   <x:si>
-    <x:t>d7a81a1f-700e-4592-bde8-5aac6b3d5acb</x:t>
+    <x:t>fef55f02-8df9-4aff-a883-7a712c1229df</x:t>
   </x:si>
   <x:si>
     <x:t>200425898</x:t>
@@ -164,7 +164,7 @@
     <x:t>21</x:t>
   </x:si>
   <x:si>
-    <x:t>4dfe8d53-f551-4399-b59b-4e34cf559a1e</x:t>
+    <x:t>38235b13-5e4e-4639-99c2-29705773bd57</x:t>
   </x:si>
   <x:si>
     <x:t>200427531</x:t>
@@ -182,10 +182,10 @@
     <x:t>26</x:t>
   </x:si>
   <x:si>
-    <x:t>6aff22f5-3ddc-4d7c-96af-feddd6fce0e8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>e86aa5e7-7fef-4bd5-864e-c6089979399f</x:t>
+    <x:t>d64a296f-c8b2-4349-af7d-0033134a7e32</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0ff0bc11-cd7a-47d9-ac23-77eb199d7f21</x:t>
   </x:si>
   <x:si>
     <x:t>200429013</x:t>
@@ -200,7 +200,7 @@
     <x:t>34312</x:t>
   </x:si>
   <x:si>
-    <x:t>d2761d5c-8e37-4895-9013-e6ccc3c92d8a</x:t>
+    <x:t>37a239e0-7ff0-4f7e-976c-e98cfe03dd39</x:t>
   </x:si>
   <x:si>
     <x:t>200429017</x:t>
@@ -215,7 +215,7 @@
     <x:t>34634</x:t>
   </x:si>
   <x:si>
-    <x:t>e479d58e-4b00-4fa4-a715-b31dd0ad3e2d</x:t>
+    <x:t>a4e371d9-f152-40ff-b3d5-841a221efeef</x:t>
   </x:si>
   <x:si>
     <x:t>200429019</x:t>
@@ -233,7 +233,7 @@
     <x:t>22</x:t>
   </x:si>
   <x:si>
-    <x:t>931aa087-3010-400a-b2a8-a970deacebc2</x:t>
+    <x:t>d1222e57-605b-47de-99ab-56b86a22d832</x:t>
   </x:si>
   <x:si>
     <x:t>200429439</x:t>
@@ -248,7 +248,7 @@
     <x:t>34585</x:t>
   </x:si>
   <x:si>
-    <x:t>aac23bf4-d026-46b0-863d-cd35af3bb6b7</x:t>
+    <x:t>2fa1868c-7ff8-4a33-aa8d-d5879c41d167</x:t>
   </x:si>
   <x:si>
     <x:t>200430242</x:t>
@@ -266,7 +266,7 @@
     <x:t>24</x:t>
   </x:si>
   <x:si>
-    <x:t>83cd2b2f-1076-4197-afd5-dc36d4174da8</x:t>
+    <x:t>dfb840b2-f579-493f-92a9-6815eeb04ebf</x:t>
   </x:si>
   <x:si>
     <x:t>200439773</x:t>
@@ -281,7 +281,7 @@
     <x:t>36072</x:t>
   </x:si>
   <x:si>
-    <x:t>dd982ad0-8af6-4590-8be3-99c1d5b7c31b</x:t>
+    <x:t>4b40b549-a467-4025-b4f0-5a722179146d</x:t>
   </x:si>
   <x:si>
     <x:t>200439932</x:t>
@@ -299,7 +299,7 @@
     <x:t>43</x:t>
   </x:si>
   <x:si>
-    <x:t>a6de6208-4032-4cce-90d1-496cae685558</x:t>
+    <x:t>e626a925-f01d-450c-90b6-82f40fab3b91</x:t>
   </x:si>
   <x:si>
     <x:t>200443399</x:t>
@@ -314,7 +314,7 @@
     <x:t>34980</x:t>
   </x:si>
   <x:si>
-    <x:t>9b548b16-749b-4da4-b4d6-ddb7b8dba18a</x:t>
+    <x:t>56033198-801a-4344-a479-098715e31a59</x:t>
   </x:si>
   <x:si>
     <x:t>200445913</x:t>
@@ -329,7 +329,7 @@
     <x:t>34166</x:t>
   </x:si>
   <x:si>
-    <x:t>b691eef5-6bc3-463a-aa66-f682c895446c</x:t>
+    <x:t>6f74ee08-04bf-4984-9112-f8e6cf6494f3</x:t>
   </x:si>
   <x:si>
     <x:t>200446535</x:t>
@@ -347,7 +347,7 @@
     <x:t>32</x:t>
   </x:si>
   <x:si>
-    <x:t>9af5d993-0ddb-4023-92a2-49ed4e4afe04</x:t>
+    <x:t>d132e12e-e3ba-49b6-8cdf-ba9acd8dad26</x:t>
   </x:si>
   <x:si>
     <x:t>2200447714</x:t>
@@ -365,10 +365,10 @@
     <x:t>0</x:t>
   </x:si>
   <x:si>
-    <x:t>027acbc2-3411-491f-9a2f-8815dd5d80d7</x:t>
-  </x:si>
-  <x:si>
-    <x:t>880e79f2-1343-4052-afb8-227d5c56940d</x:t>
+    <x:t>7708f00d-3a9a-45a9-800e-a20b7459187e</x:t>
+  </x:si>
+  <x:si>
+    <x:t>987bc6b7-960b-40c7-a5db-84441a2e8ca1</x:t>
   </x:si>
   <x:si>
     <x:t>200447184</x:t>
@@ -383,7 +383,7 @@
     <x:t>35822</x:t>
   </x:si>
   <x:si>
-    <x:t>49ee1334-3fc8-467e-9c51-08660089be47</x:t>
+    <x:t>450a8974-8bbf-4b3d-b687-0e0996468ce5</x:t>
   </x:si>
   <x:si>
     <x:t>200447197</x:t>
@@ -398,7 +398,7 @@
     <x:t>35535</x:t>
   </x:si>
   <x:si>
-    <x:t>29a7baa3-1b37-46a1-ac4a-791f2e6bbca5</x:t>
+    <x:t>49aa0019-dc8a-42c9-9ddd-458a5c36bc6e</x:t>
   </x:si>
   <x:si>
     <x:t>200447261</x:t>
@@ -413,7 +413,7 @@
     <x:t>34154</x:t>
   </x:si>
   <x:si>
-    <x:t>8e675fc8-8ef3-4778-b467-1c8730da9d59</x:t>
+    <x:t>825b1115-4048-4a0b-908f-33652eeed4d7</x:t>
   </x:si>
   <x:si>
     <x:t>200447330</x:t>
@@ -431,7 +431,7 @@
     <x:t>27</x:t>
   </x:si>
   <x:si>
-    <x:t>e0ea6d09-f201-4442-979c-aec05e0396c6</x:t>
+    <x:t>8b0a0aa1-b8dd-4f0f-8c21-44437a9fb1ae</x:t>
   </x:si>
   <x:si>
     <x:t>200447599</x:t>
@@ -446,7 +446,7 @@
     <x:t>34599</x:t>
   </x:si>
   <x:si>
-    <x:t>4e6944a8-aa7d-4217-94e7-37fa4b7ec738</x:t>
+    <x:t>36590960-9a79-4b82-a30e-401a5d927023</x:t>
   </x:si>
   <x:si>
     <x:t>200447744</x:t>
@@ -461,7 +461,7 @@
     <x:t>34099</x:t>
   </x:si>
   <x:si>
-    <x:t>1253add6-81d9-4154-9aec-e409ce52a79f</x:t>
+    <x:t>36b1b2d0-1c05-4a9d-b566-8e223dca9ba0</x:t>
   </x:si>
   <x:si>
     <x:t>200447887</x:t>
@@ -476,7 +476,7 @@
     <x:t>35824</x:t>
   </x:si>
   <x:si>
-    <x:t>2f2d3d3d-20fb-4e61-b83b-f09c532e8459</x:t>
+    <x:t>03c240d7-b698-4065-a026-e9deeb7aa3df</x:t>
   </x:si>
   <x:si>
     <x:t>200448232</x:t>
@@ -491,7 +491,7 @@
     <x:t>35425</x:t>
   </x:si>
   <x:si>
-    <x:t>c7ea45b9-e5eb-480f-a03f-7a427063fe90</x:t>
+    <x:t>31766af9-25a1-43ca-8d49-686d19594f05</x:t>
   </x:si>
   <x:si>
     <x:t>200449068</x:t>
@@ -512,7 +512,7 @@
     <x:t>39</x:t>
   </x:si>
   <x:si>
-    <x:t>a1ec5d99-b17e-4139-b02c-f4c2f14dad64</x:t>
+    <x:t>c7bf6b1f-df87-412e-bb55-cb3408136802</x:t>
   </x:si>
   <x:si>
     <x:t>200449112</x:t>
@@ -527,7 +527,7 @@
     <x:t>34569</x:t>
   </x:si>
   <x:si>
-    <x:t>d628e667-b13e-4020-b8c4-0f9c6a85cc2e</x:t>
+    <x:t>6d91d66e-de0b-4b32-afcf-d684a0c10b7a</x:t>
   </x:si>
   <x:si>
     <x:t>200449872</x:t>
@@ -542,7 +542,7 @@
     <x:t>34234</x:t>
   </x:si>
   <x:si>
-    <x:t>8790fae2-1fc1-4435-8f6b-9f5995c8d696</x:t>
+    <x:t>10dd97b5-f366-47fa-9bbd-dbb02d3099c4</x:t>
   </x:si>
   <x:si>
     <x:t>200450261</x:t>
@@ -557,7 +557,7 @@
     <x:t>34439</x:t>
   </x:si>
   <x:si>
-    <x:t>2b247f9e-12a3-4aaa-ac13-757bc6dc2324</x:t>
+    <x:t>7a709a23-4a70-4752-8d4c-d9bf451f06e1</x:t>
   </x:si>
   <x:si>
     <x:t>200450333</x:t>
@@ -572,7 +572,7 @@
     <x:t>33969</x:t>
   </x:si>
   <x:si>
-    <x:t>a135d6d0-5377-455b-a9ee-768e9b6dbd7b</x:t>
+    <x:t>ac3676c8-51c7-4924-96ad-273ef8c1cbe1</x:t>
   </x:si>
   <x:si>
     <x:t>200450515</x:t>
@@ -587,7 +587,7 @@
     <x:t>34533</x:t>
   </x:si>
   <x:si>
-    <x:t>1fc3af12-8bb3-471e-acc1-c63fb970ff55</x:t>
+    <x:t>ed4ee6fb-4e5e-4b26-9491-40bb7dcb91c0</x:t>
   </x:si>
   <x:si>
     <x:t>200450550</x:t>
@@ -602,7 +602,7 @@
     <x:t>35764</x:t>
   </x:si>
   <x:si>
-    <x:t>b5853849-cde3-421c-9b40-c4de33a2fe94</x:t>
+    <x:t>83d2762e-c235-4b27-9b67-af8684ba1922</x:t>
   </x:si>
   <x:si>
     <x:t>200450635</x:t>
@@ -614,7 +614,7 @@
     <x:t>35470</x:t>
   </x:si>
   <x:si>
-    <x:t>ca2b8c30-079b-47e3-bb0e-afdb8d7af0c9</x:t>
+    <x:t>0e845011-703c-4aaa-8fc6-09cd258a5024</x:t>
   </x:si>
   <x:si>
     <x:t>200450730</x:t>
@@ -626,7 +626,7 @@
     <x:t>35941</x:t>
   </x:si>
   <x:si>
-    <x:t>69bf9cfe-f495-499e-a89b-9baf5e3773b4</x:t>
+    <x:t>26068c62-5278-448e-903d-ce66a1f11cd3</x:t>
   </x:si>
   <x:si>
     <x:t>200451605</x:t>

</xml_diff>